<commit_message>
contact icons and some changes
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurusaishreeshtirumalla/Desktop/pyproj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurusaishreeshtirumalla/Desktop/Emailbot-ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A71A2-C263-E947-A8B1-D62F396DB0DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D1DC8B-799C-AD49-BE93-615192D95F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{36E2957E-6CDE-3C4D-9373-6583AB28DC48}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{36E2957E-6CDE-3C4D-9373-6583AB28DC48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,10 +456,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -467,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -487,7 +487,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{85D7A331-49F1-7A45-A91D-D7DBB4AB1BA0}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{6F9EA0E3-1BD4-A348-A5A0-8F9940F028C5}"/>
+    <hyperlink ref="C3" r:id="rId2" display="guru.sai.shreesh@gmail.com" xr:uid="{6F9EA0E3-1BD4-A348-A5A0-8F9940F028C5}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{9A4786B4-F0F3-444C-8F6A-205D36652944}"/>
     <hyperlink ref="C4" r:id="rId4" display="gojo.testing123@gmail.com" xr:uid="{98DF030E-00B4-3B4E-B556-373C63892DC5}"/>
   </hyperlinks>

</xml_diff>